<commit_message>
Censuses DB adapted to MySQL
</commit_message>
<xml_diff>
--- a/censuses_I1b/src/test/java/es/uniovi/asw/jdbc/votersXSSFReaderTest.xlsx
+++ b/censuses_I1b/src/test/java/es/uniovi/asw/jdbc/votersXSSFReaderTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uo237633\IdeaProjects\censuses_i1b\src\test\java\es\uniovi\asw\jdbc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\ASW\practicas\trabajos\entrega final\Voting_I1b\censuses_I1b\src\test\java\es\uniovi\asw\jdbc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>nombre</t>
   </si>
@@ -56,12 +56,6 @@
     <t>22222J</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>Pepe</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
   </si>
   <si>
     <t>pepe@gmail.com</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
 </sst>
 </file>
@@ -121,7 +112,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -138,7 +129,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -406,7 +397,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
@@ -438,8 +429,8 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -452,22 +443,22 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+      <c r="D4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>